<commit_message>
updated team_list for wisconsin
</commit_message>
<xml_diff>
--- a/readthis.xlsx
+++ b/readthis.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="final" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
   <si>
     <t>high</t>
   </si>
@@ -164,8 +165,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -181,15 +186,19 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8379,8 +8388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14602,6 +14611,4491 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="1.5" customWidth="1"/>
+    <col min="11" max="11" width="1.1640625" customWidth="1"/>
+    <col min="21" max="21" width="1.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="45">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="e">
+        <f>'[1]shot analysis'!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" t="e">
+        <f>'[1]shot analysis'!M3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D3" t="e">
+        <f>'[1]shot analysis'!N3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E3" t="e">
+        <f>'[1]shot analysis'!O3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" t="e">
+        <f>'[1]shot analysis'!AA3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H3" t="e">
+        <f>'[1]shot analysis'!AB3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" t="e">
+        <f>'[1]shot analysis'!AC3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" t="e">
+        <f>'[1]shot analysis'!AD3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L3" t="e">
+        <f>[1]portcullis!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M3" t="e">
+        <f>'[1]cheval de frise'!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N3" t="e">
+        <f>[1]moat!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O3" t="e">
+        <f>[1]ramparts!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P3" t="e">
+        <f>[1]drawbridge!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q3" t="e">
+        <f>'[1]sally port'!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R3" t="e">
+        <f>'[1]rock wall'!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S3" t="e">
+        <f>'[1]rough terrain'!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T3" t="e">
+        <f>[1]lowbar!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V3" t="e">
+        <f>[1]climb!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W3" t="e">
+        <f>[1]rip!L2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4">
+        <v>192</v>
+      </c>
+      <c r="B4" t="e">
+        <f>'[1]shot analysis'!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" t="e">
+        <f>'[1]shot analysis'!M4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D4" t="e">
+        <f>'[1]shot analysis'!N4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E4" t="e">
+        <f>'[1]shot analysis'!O4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
+        <f>'[1]shot analysis'!AA4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" t="e">
+        <f>'[1]shot analysis'!AB4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I4" t="e">
+        <f>'[1]shot analysis'!AC4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" t="e">
+        <f>'[1]shot analysis'!AD4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L4" t="e">
+        <f>[1]portcullis!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4" t="e">
+        <f>'[1]cheval de frise'!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N4" t="e">
+        <f>[1]moat!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O4" t="e">
+        <f>[1]ramparts!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P4" t="e">
+        <f>[1]drawbridge!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q4" t="e">
+        <f>'[1]sally port'!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R4" t="e">
+        <f>'[1]rock wall'!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S4" t="e">
+        <f>'[1]rough terrain'!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T4" t="e">
+        <f>[1]lowbar!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V4" t="e">
+        <f>[1]climb!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W4" t="e">
+        <f>[1]rip!L3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="e">
+        <f>'[1]shot analysis'!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" t="e">
+        <f>'[1]shot analysis'!M5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D5" t="e">
+        <f>'[1]shot analysis'!N5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E5" t="e">
+        <f>'[1]shot analysis'!O5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" t="e">
+        <f>'[1]shot analysis'!AA5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" t="e">
+        <f>'[1]shot analysis'!AB5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5" t="e">
+        <f>'[1]shot analysis'!AC5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" t="e">
+        <f>'[1]shot analysis'!AD5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L5" t="e">
+        <f>[1]portcullis!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" t="e">
+        <f>'[1]cheval de frise'!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N5" t="e">
+        <f>[1]moat!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O5" t="e">
+        <f>[1]ramparts!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" t="e">
+        <f>[1]drawbridge!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q5" t="e">
+        <f>'[1]sally port'!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R5" t="e">
+        <f>'[1]rock wall'!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S5" t="e">
+        <f>'[1]rough terrain'!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T5" t="e">
+        <f>[1]lowbar!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V5" t="e">
+        <f>[1]climb!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W5" t="e">
+        <f>[1]rip!L4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="e">
+        <f>'[1]shot analysis'!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" t="e">
+        <f>'[1]shot analysis'!M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D6" t="e">
+        <f>'[1]shot analysis'!N6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E6" t="e">
+        <f>'[1]shot analysis'!O6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" t="e">
+        <f>'[1]shot analysis'!AA6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" t="e">
+        <f>'[1]shot analysis'!AB6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6" t="e">
+        <f>'[1]shot analysis'!AC6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" t="e">
+        <f>'[1]shot analysis'!AD6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L6" t="e">
+        <f>[1]portcullis!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6" t="e">
+        <f>'[1]cheval de frise'!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" t="e">
+        <f>[1]moat!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O6" t="e">
+        <f>[1]ramparts!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" t="e">
+        <f>[1]drawbridge!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q6" t="e">
+        <f>'[1]sally port'!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R6" t="e">
+        <f>'[1]rock wall'!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S6" t="e">
+        <f>'[1]rough terrain'!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T6" t="e">
+        <f>[1]lowbar!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V6" t="e">
+        <f>[1]climb!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W6" t="e">
+        <f>[1]rip!L5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="e">
+        <f>'[1]shot analysis'!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" t="e">
+        <f>'[1]shot analysis'!M7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D7" t="e">
+        <f>'[1]shot analysis'!N7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E7" t="e">
+        <f>'[1]shot analysis'!O7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" t="e">
+        <f>'[1]shot analysis'!AA7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" t="e">
+        <f>'[1]shot analysis'!AB7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" t="e">
+        <f>'[1]shot analysis'!AC7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" t="e">
+        <f>'[1]shot analysis'!AD7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L7" t="e">
+        <f>[1]portcullis!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" t="e">
+        <f>'[1]cheval de frise'!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" t="e">
+        <f>[1]moat!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O7" t="e">
+        <f>[1]ramparts!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" t="e">
+        <f>[1]drawbridge!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q7" t="e">
+        <f>'[1]sally port'!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R7" t="e">
+        <f>'[1]rock wall'!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S7" t="e">
+        <f>'[1]rough terrain'!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T7" t="e">
+        <f>[1]lowbar!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V7" t="e">
+        <f>[1]climb!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W7" t="e">
+        <f>[1]rip!L6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="e">
+        <f>'[1]shot analysis'!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" t="e">
+        <f>'[1]shot analysis'!M8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D8" t="e">
+        <f>'[1]shot analysis'!N8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E8" t="e">
+        <f>'[1]shot analysis'!O8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" t="e">
+        <f>'[1]shot analysis'!AA8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" t="e">
+        <f>'[1]shot analysis'!AB8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" t="e">
+        <f>'[1]shot analysis'!AC8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" t="e">
+        <f>'[1]shot analysis'!AD8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L8" t="e">
+        <f>[1]portcullis!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" t="e">
+        <f>'[1]cheval de frise'!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" t="e">
+        <f>[1]moat!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" t="e">
+        <f>[1]ramparts!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" t="e">
+        <f>[1]drawbridge!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q8" t="e">
+        <f>'[1]sally port'!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R8" t="e">
+        <f>'[1]rock wall'!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S8" t="e">
+        <f>'[1]rough terrain'!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T8" t="e">
+        <f>[1]lowbar!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V8" t="e">
+        <f>[1]climb!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W8" t="e">
+        <f>[1]rip!L7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="e">
+        <f>'[1]shot analysis'!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" t="e">
+        <f>'[1]shot analysis'!M9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D9" t="e">
+        <f>'[1]shot analysis'!N9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E9" t="e">
+        <f>'[1]shot analysis'!O9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" t="e">
+        <f>'[1]shot analysis'!AA9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" t="e">
+        <f>'[1]shot analysis'!AB9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" t="e">
+        <f>'[1]shot analysis'!AC9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" t="e">
+        <f>'[1]shot analysis'!AD9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L9" t="e">
+        <f>[1]portcullis!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" t="e">
+        <f>'[1]cheval de frise'!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" t="e">
+        <f>[1]moat!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" t="e">
+        <f>[1]ramparts!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" t="e">
+        <f>[1]drawbridge!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q9" t="e">
+        <f>'[1]sally port'!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" t="e">
+        <f>'[1]rock wall'!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S9" t="e">
+        <f>'[1]rough terrain'!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T9" t="e">
+        <f>[1]lowbar!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V9" t="e">
+        <f>[1]climb!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W9" t="e">
+        <f>[1]rip!L8</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="e">
+        <f>'[1]shot analysis'!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" t="e">
+        <f>'[1]shot analysis'!M10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D10" t="e">
+        <f>'[1]shot analysis'!N10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" t="e">
+        <f>'[1]shot analysis'!O10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" t="e">
+        <f>'[1]shot analysis'!AA10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" t="e">
+        <f>'[1]shot analysis'!AB10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" t="e">
+        <f>'[1]shot analysis'!AC10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" t="e">
+        <f>'[1]shot analysis'!AD10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L10" t="e">
+        <f>[1]portcullis!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10" t="e">
+        <f>'[1]cheval de frise'!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" t="e">
+        <f>[1]moat!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O10" t="e">
+        <f>[1]ramparts!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" t="e">
+        <f>[1]drawbridge!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q10" t="e">
+        <f>'[1]sally port'!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R10" t="e">
+        <f>'[1]rock wall'!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S10" t="e">
+        <f>'[1]rough terrain'!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T10" t="e">
+        <f>[1]lowbar!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V10" t="e">
+        <f>[1]climb!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W10" t="e">
+        <f>[1]rip!L9</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="e">
+        <f>'[1]shot analysis'!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" t="e">
+        <f>'[1]shot analysis'!M11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D11" t="e">
+        <f>'[1]shot analysis'!N11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" t="e">
+        <f>'[1]shot analysis'!O11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" t="e">
+        <f>'[1]shot analysis'!AA11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" t="e">
+        <f>'[1]shot analysis'!AB11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" t="e">
+        <f>'[1]shot analysis'!AC11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" t="e">
+        <f>'[1]shot analysis'!AD11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L11" t="e">
+        <f>[1]portcullis!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" t="e">
+        <f>'[1]cheval de frise'!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" t="e">
+        <f>[1]moat!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O11" t="e">
+        <f>[1]ramparts!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" t="e">
+        <f>[1]drawbridge!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q11" t="e">
+        <f>'[1]sally port'!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R11" t="e">
+        <f>'[1]rock wall'!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S11" t="e">
+        <f>'[1]rough terrain'!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T11" t="e">
+        <f>[1]lowbar!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V11" t="e">
+        <f>[1]climb!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W11" t="e">
+        <f>[1]rip!L10</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="e">
+        <f>'[1]shot analysis'!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C12" t="e">
+        <f>'[1]shot analysis'!M12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D12" t="e">
+        <f>'[1]shot analysis'!N12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12" t="e">
+        <f>'[1]shot analysis'!O12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" t="e">
+        <f>'[1]shot analysis'!AA12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" t="e">
+        <f>'[1]shot analysis'!AB12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" t="e">
+        <f>'[1]shot analysis'!AC12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" t="e">
+        <f>'[1]shot analysis'!AD12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L12" t="e">
+        <f>[1]portcullis!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" t="e">
+        <f>'[1]cheval de frise'!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N12" t="e">
+        <f>[1]moat!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O12" t="e">
+        <f>[1]ramparts!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" t="e">
+        <f>[1]drawbridge!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q12" t="e">
+        <f>'[1]sally port'!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R12" t="e">
+        <f>'[1]rock wall'!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S12" t="e">
+        <f>'[1]rough terrain'!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T12" t="e">
+        <f>[1]lowbar!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V12" t="e">
+        <f>[1]climb!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W12" t="e">
+        <f>[1]rip!L11</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="e">
+        <f>'[1]shot analysis'!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C13" t="e">
+        <f>'[1]shot analysis'!M13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D13" t="e">
+        <f>'[1]shot analysis'!N13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" t="e">
+        <f>'[1]shot analysis'!O13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" t="e">
+        <f>'[1]shot analysis'!AA13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" t="e">
+        <f>'[1]shot analysis'!AB13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" t="e">
+        <f>'[1]shot analysis'!AC13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" t="e">
+        <f>'[1]shot analysis'!AD13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13" t="e">
+        <f>[1]portcullis!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" t="e">
+        <f>'[1]cheval de frise'!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" t="e">
+        <f>[1]moat!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" t="e">
+        <f>[1]ramparts!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" t="e">
+        <f>[1]drawbridge!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q13" t="e">
+        <f>'[1]sally port'!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R13" t="e">
+        <f>'[1]rock wall'!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S13" t="e">
+        <f>'[1]rough terrain'!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T13" t="e">
+        <f>[1]lowbar!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V13" t="e">
+        <f>[1]climb!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W13" t="e">
+        <f>[1]rip!L12</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="e">
+        <f>'[1]shot analysis'!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C14" t="e">
+        <f>'[1]shot analysis'!M14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D14" t="e">
+        <f>'[1]shot analysis'!N14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" t="e">
+        <f>'[1]shot analysis'!O14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" t="e">
+        <f>'[1]shot analysis'!AA14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" t="e">
+        <f>'[1]shot analysis'!AB14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" t="e">
+        <f>'[1]shot analysis'!AC14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" t="e">
+        <f>'[1]shot analysis'!AD14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L14" t="e">
+        <f>[1]portcullis!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" t="e">
+        <f>'[1]cheval de frise'!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N14" t="e">
+        <f>[1]moat!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O14" t="e">
+        <f>[1]ramparts!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P14" t="e">
+        <f>[1]drawbridge!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q14" t="e">
+        <f>'[1]sally port'!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R14" t="e">
+        <f>'[1]rock wall'!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S14" t="e">
+        <f>'[1]rough terrain'!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T14" t="e">
+        <f>[1]lowbar!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V14" t="e">
+        <f>[1]climb!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W14" t="e">
+        <f>[1]rip!L13</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="e">
+        <f>'[1]shot analysis'!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C15" t="e">
+        <f>'[1]shot analysis'!M15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" t="e">
+        <f>'[1]shot analysis'!N15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" t="e">
+        <f>'[1]shot analysis'!O15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" t="e">
+        <f>'[1]shot analysis'!AA15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" t="e">
+        <f>'[1]shot analysis'!AB15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" t="e">
+        <f>'[1]shot analysis'!AC15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" t="e">
+        <f>'[1]shot analysis'!AD15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" t="e">
+        <f>[1]portcullis!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" t="e">
+        <f>'[1]cheval de frise'!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" t="e">
+        <f>[1]moat!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" t="e">
+        <f>[1]ramparts!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" t="e">
+        <f>[1]drawbridge!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q15" t="e">
+        <f>'[1]sally port'!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R15" t="e">
+        <f>'[1]rock wall'!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S15" t="e">
+        <f>'[1]rough terrain'!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T15" t="e">
+        <f>[1]lowbar!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V15" t="e">
+        <f>[1]climb!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W15" t="e">
+        <f>[1]rip!L14</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="e">
+        <f>'[1]shot analysis'!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C16" t="e">
+        <f>'[1]shot analysis'!M16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D16" t="e">
+        <f>'[1]shot analysis'!N16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" t="e">
+        <f>'[1]shot analysis'!O16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" t="e">
+        <f>'[1]shot analysis'!AA16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" t="e">
+        <f>'[1]shot analysis'!AB16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" t="e">
+        <f>'[1]shot analysis'!AC16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" t="e">
+        <f>'[1]shot analysis'!AD16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L16" t="e">
+        <f>[1]portcullis!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" t="e">
+        <f>'[1]cheval de frise'!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" t="e">
+        <f>[1]moat!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" t="e">
+        <f>[1]ramparts!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" t="e">
+        <f>[1]drawbridge!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q16" t="e">
+        <f>'[1]sally port'!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R16" t="e">
+        <f>'[1]rock wall'!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S16" t="e">
+        <f>'[1]rough terrain'!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T16" t="e">
+        <f>[1]lowbar!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V16" t="e">
+        <f>[1]climb!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W16" t="e">
+        <f>[1]rip!L15</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="e">
+        <f>'[1]shot analysis'!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17" t="e">
+        <f>'[1]shot analysis'!M17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D17" t="e">
+        <f>'[1]shot analysis'!N17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" t="e">
+        <f>'[1]shot analysis'!O17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" t="e">
+        <f>'[1]shot analysis'!AA17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" t="e">
+        <f>'[1]shot analysis'!AB17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" t="e">
+        <f>'[1]shot analysis'!AC17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" t="e">
+        <f>'[1]shot analysis'!AD17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" t="e">
+        <f>[1]portcullis!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" t="e">
+        <f>'[1]cheval de frise'!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N17" t="e">
+        <f>[1]moat!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" t="e">
+        <f>[1]ramparts!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" t="e">
+        <f>[1]drawbridge!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q17" t="e">
+        <f>'[1]sally port'!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R17" t="e">
+        <f>'[1]rock wall'!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S17" t="e">
+        <f>'[1]rough terrain'!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T17" t="e">
+        <f>[1]lowbar!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V17" t="e">
+        <f>[1]climb!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W17" t="e">
+        <f>[1]rip!L16</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="e">
+        <f>'[1]shot analysis'!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C18" t="e">
+        <f>'[1]shot analysis'!M18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D18" t="e">
+        <f>'[1]shot analysis'!N18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" t="e">
+        <f>'[1]shot analysis'!O18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" t="e">
+        <f>'[1]shot analysis'!AA18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" t="e">
+        <f>'[1]shot analysis'!AB18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" t="e">
+        <f>'[1]shot analysis'!AC18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" t="e">
+        <f>'[1]shot analysis'!AD18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" t="e">
+        <f>[1]portcullis!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" t="e">
+        <f>'[1]cheval de frise'!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" t="e">
+        <f>[1]moat!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" t="e">
+        <f>[1]ramparts!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" t="e">
+        <f>[1]drawbridge!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q18" t="e">
+        <f>'[1]sally port'!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R18" t="e">
+        <f>'[1]rock wall'!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S18" t="e">
+        <f>'[1]rough terrain'!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T18" t="e">
+        <f>[1]lowbar!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V18" t="e">
+        <f>[1]climb!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W18" t="e">
+        <f>[1]rip!L17</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="e">
+        <f>'[1]shot analysis'!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C19" t="e">
+        <f>'[1]shot analysis'!M19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D19" t="e">
+        <f>'[1]shot analysis'!N19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" t="e">
+        <f>'[1]shot analysis'!O19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" t="e">
+        <f>'[1]shot analysis'!AA19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" t="e">
+        <f>'[1]shot analysis'!AB19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" t="e">
+        <f>'[1]shot analysis'!AC19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" t="e">
+        <f>'[1]shot analysis'!AD19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L19" t="e">
+        <f>[1]portcullis!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" t="e">
+        <f>'[1]cheval de frise'!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" t="e">
+        <f>[1]moat!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" t="e">
+        <f>[1]ramparts!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" t="e">
+        <f>[1]drawbridge!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" t="e">
+        <f>'[1]sally port'!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R19" t="e">
+        <f>'[1]rock wall'!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S19" t="e">
+        <f>'[1]rough terrain'!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T19" t="e">
+        <f>[1]lowbar!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V19" t="e">
+        <f>[1]climb!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W19" t="e">
+        <f>[1]rip!L18</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="e">
+        <f>'[1]shot analysis'!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C20" t="e">
+        <f>'[1]shot analysis'!M20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D20" t="e">
+        <f>'[1]shot analysis'!N20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E20" t="e">
+        <f>'[1]shot analysis'!O20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" t="e">
+        <f>'[1]shot analysis'!AA20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" t="e">
+        <f>'[1]shot analysis'!AB20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" t="e">
+        <f>'[1]shot analysis'!AC20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" t="e">
+        <f>'[1]shot analysis'!AD20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L20" t="e">
+        <f>[1]portcullis!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20" t="e">
+        <f>'[1]cheval de frise'!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" t="e">
+        <f>[1]moat!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" t="e">
+        <f>[1]ramparts!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" t="e">
+        <f>[1]drawbridge!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q20" t="e">
+        <f>'[1]sally port'!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R20" t="e">
+        <f>'[1]rock wall'!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S20" t="e">
+        <f>'[1]rough terrain'!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T20" t="e">
+        <f>[1]lowbar!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V20" t="e">
+        <f>[1]climb!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W20" t="e">
+        <f>[1]rip!L19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="e">
+        <f>'[1]shot analysis'!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C21" t="e">
+        <f>'[1]shot analysis'!M21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D21" t="e">
+        <f>'[1]shot analysis'!N21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E21" t="e">
+        <f>'[1]shot analysis'!O21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" t="e">
+        <f>'[1]shot analysis'!AA21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" t="e">
+        <f>'[1]shot analysis'!AB21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" t="e">
+        <f>'[1]shot analysis'!AC21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" t="e">
+        <f>'[1]shot analysis'!AD21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L21" t="e">
+        <f>[1]portcullis!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21" t="e">
+        <f>'[1]cheval de frise'!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" t="e">
+        <f>[1]moat!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" t="e">
+        <f>[1]ramparts!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" t="e">
+        <f>[1]drawbridge!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q21" t="e">
+        <f>'[1]sally port'!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R21" t="e">
+        <f>'[1]rock wall'!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S21" t="e">
+        <f>'[1]rough terrain'!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T21" t="e">
+        <f>[1]lowbar!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V21" t="e">
+        <f>[1]climb!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W21" t="e">
+        <f>[1]rip!L20</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="e">
+        <f>'[1]shot analysis'!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C22" t="e">
+        <f>'[1]shot analysis'!M22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D22" t="e">
+        <f>'[1]shot analysis'!N22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E22" t="e">
+        <f>'[1]shot analysis'!O22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" t="e">
+        <f>'[1]shot analysis'!AA22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" t="e">
+        <f>'[1]shot analysis'!AB22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" t="e">
+        <f>'[1]shot analysis'!AC22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" t="e">
+        <f>'[1]shot analysis'!AD22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L22" t="e">
+        <f>[1]portcullis!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M22" t="e">
+        <f>'[1]cheval de frise'!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N22" t="e">
+        <f>[1]moat!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" t="e">
+        <f>[1]ramparts!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P22" t="e">
+        <f>[1]drawbridge!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q22" t="e">
+        <f>'[1]sally port'!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R22" t="e">
+        <f>'[1]rock wall'!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S22" t="e">
+        <f>'[1]rough terrain'!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T22" t="e">
+        <f>[1]lowbar!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V22" t="e">
+        <f>[1]climb!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W22" t="e">
+        <f>[1]rip!L21</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="e">
+        <f>'[1]shot analysis'!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C23" t="e">
+        <f>'[1]shot analysis'!M23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D23" t="e">
+        <f>'[1]shot analysis'!N23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" t="e">
+        <f>'[1]shot analysis'!O23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" t="e">
+        <f>'[1]shot analysis'!AA23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" t="e">
+        <f>'[1]shot analysis'!AB23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" t="e">
+        <f>'[1]shot analysis'!AC23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23" t="e">
+        <f>'[1]shot analysis'!AD23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L23" t="e">
+        <f>[1]portcullis!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" t="e">
+        <f>'[1]cheval de frise'!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" t="e">
+        <f>[1]moat!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O23" t="e">
+        <f>[1]ramparts!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P23" t="e">
+        <f>[1]drawbridge!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q23" t="e">
+        <f>'[1]sally port'!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R23" t="e">
+        <f>'[1]rock wall'!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S23" t="e">
+        <f>'[1]rough terrain'!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T23" t="e">
+        <f>[1]lowbar!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V23" t="e">
+        <f>[1]climb!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W23" t="e">
+        <f>[1]rip!L22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="e">
+        <f>'[1]shot analysis'!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C24" t="e">
+        <f>'[1]shot analysis'!M24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D24" t="e">
+        <f>'[1]shot analysis'!N24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E24" t="e">
+        <f>'[1]shot analysis'!O24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G24" t="e">
+        <f>'[1]shot analysis'!AA24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H24" t="e">
+        <f>'[1]shot analysis'!AB24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" t="e">
+        <f>'[1]shot analysis'!AC24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J24" t="e">
+        <f>'[1]shot analysis'!AD24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L24" t="e">
+        <f>[1]portcullis!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M24" t="e">
+        <f>'[1]cheval de frise'!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N24" t="e">
+        <f>[1]moat!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O24" t="e">
+        <f>[1]ramparts!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P24" t="e">
+        <f>[1]drawbridge!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q24" t="e">
+        <f>'[1]sally port'!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R24" t="e">
+        <f>'[1]rock wall'!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S24" t="e">
+        <f>'[1]rough terrain'!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T24" t="e">
+        <f>[1]lowbar!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V24" t="e">
+        <f>[1]climb!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W24" t="e">
+        <f>[1]rip!L23</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="e">
+        <f>'[1]shot analysis'!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C25" t="e">
+        <f>'[1]shot analysis'!M25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D25" t="e">
+        <f>'[1]shot analysis'!N25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E25" t="e">
+        <f>'[1]shot analysis'!O25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G25" t="e">
+        <f>'[1]shot analysis'!AA25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H25" t="e">
+        <f>'[1]shot analysis'!AB25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" t="e">
+        <f>'[1]shot analysis'!AC25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J25" t="e">
+        <f>'[1]shot analysis'!AD25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L25" t="e">
+        <f>[1]portcullis!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25" t="e">
+        <f>'[1]cheval de frise'!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N25" t="e">
+        <f>[1]moat!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O25" t="e">
+        <f>[1]ramparts!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P25" t="e">
+        <f>[1]drawbridge!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q25" t="e">
+        <f>'[1]sally port'!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R25" t="e">
+        <f>'[1]rock wall'!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S25" t="e">
+        <f>'[1]rough terrain'!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T25" t="e">
+        <f>[1]lowbar!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V25" t="e">
+        <f>[1]climb!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W25" t="e">
+        <f>[1]rip!L24</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="e">
+        <f>'[1]shot analysis'!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C26" t="e">
+        <f>'[1]shot analysis'!M26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D26" t="e">
+        <f>'[1]shot analysis'!N26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E26" t="e">
+        <f>'[1]shot analysis'!O26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G26" t="e">
+        <f>'[1]shot analysis'!AA26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H26" t="e">
+        <f>'[1]shot analysis'!AB26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" t="e">
+        <f>'[1]shot analysis'!AC26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J26" t="e">
+        <f>'[1]shot analysis'!AD26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L26" t="e">
+        <f>[1]portcullis!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M26" t="e">
+        <f>'[1]cheval de frise'!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N26" t="e">
+        <f>[1]moat!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O26" t="e">
+        <f>[1]ramparts!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P26" t="e">
+        <f>[1]drawbridge!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q26" t="e">
+        <f>'[1]sally port'!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R26" t="e">
+        <f>'[1]rock wall'!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S26" t="e">
+        <f>'[1]rough terrain'!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T26" t="e">
+        <f>[1]lowbar!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V26" t="e">
+        <f>[1]climb!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W26" t="e">
+        <f>[1]rip!L25</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="e">
+        <f>'[1]shot analysis'!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C27" t="e">
+        <f>'[1]shot analysis'!M27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D27" t="e">
+        <f>'[1]shot analysis'!N27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E27" t="e">
+        <f>'[1]shot analysis'!O27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G27" t="e">
+        <f>'[1]shot analysis'!AA27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H27" t="e">
+        <f>'[1]shot analysis'!AB27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" t="e">
+        <f>'[1]shot analysis'!AC27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J27" t="e">
+        <f>'[1]shot analysis'!AD27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L27" t="e">
+        <f>[1]portcullis!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M27" t="e">
+        <f>'[1]cheval de frise'!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N27" t="e">
+        <f>[1]moat!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O27" t="e">
+        <f>[1]ramparts!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P27" t="e">
+        <f>[1]drawbridge!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q27" t="e">
+        <f>'[1]sally port'!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R27" t="e">
+        <f>'[1]rock wall'!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S27" t="e">
+        <f>'[1]rough terrain'!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T27" t="e">
+        <f>[1]lowbar!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V27" t="e">
+        <f>[1]climb!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W27" t="e">
+        <f>[1]rip!L26</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="e">
+        <f>'[1]shot analysis'!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C28" t="e">
+        <f>'[1]shot analysis'!M28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D28" t="e">
+        <f>'[1]shot analysis'!N28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E28" t="e">
+        <f>'[1]shot analysis'!O28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G28" t="e">
+        <f>'[1]shot analysis'!AA28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" t="e">
+        <f>'[1]shot analysis'!AB28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" t="e">
+        <f>'[1]shot analysis'!AC28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" t="e">
+        <f>'[1]shot analysis'!AD28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L28" t="e">
+        <f>[1]portcullis!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M28" t="e">
+        <f>'[1]cheval de frise'!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N28" t="e">
+        <f>[1]moat!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O28" t="e">
+        <f>[1]ramparts!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P28" t="e">
+        <f>[1]drawbridge!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q28" t="e">
+        <f>'[1]sally port'!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R28" t="e">
+        <f>'[1]rock wall'!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S28" t="e">
+        <f>'[1]rough terrain'!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T28" t="e">
+        <f>[1]lowbar!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V28" t="e">
+        <f>[1]climb!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W28" t="e">
+        <f>[1]rip!L27</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="e">
+        <f>'[1]shot analysis'!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C29" t="e">
+        <f>'[1]shot analysis'!M29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D29" t="e">
+        <f>'[1]shot analysis'!N29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E29" t="e">
+        <f>'[1]shot analysis'!O29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" t="e">
+        <f>'[1]shot analysis'!AA29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" t="e">
+        <f>'[1]shot analysis'!AB29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" t="e">
+        <f>'[1]shot analysis'!AC29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29" t="e">
+        <f>'[1]shot analysis'!AD29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L29" t="e">
+        <f>[1]portcullis!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29" t="e">
+        <f>'[1]cheval de frise'!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N29" t="e">
+        <f>[1]moat!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O29" t="e">
+        <f>[1]ramparts!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P29" t="e">
+        <f>[1]drawbridge!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q29" t="e">
+        <f>'[1]sally port'!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R29" t="e">
+        <f>'[1]rock wall'!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S29" t="e">
+        <f>'[1]rough terrain'!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T29" t="e">
+        <f>[1]lowbar!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V29" t="e">
+        <f>[1]climb!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W29" t="e">
+        <f>[1]rip!L28</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="e">
+        <f>'[1]shot analysis'!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C30" t="e">
+        <f>'[1]shot analysis'!M30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D30" t="e">
+        <f>'[1]shot analysis'!N30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E30" t="e">
+        <f>'[1]shot analysis'!O30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G30" t="e">
+        <f>'[1]shot analysis'!AA30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" t="e">
+        <f>'[1]shot analysis'!AB30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" t="e">
+        <f>'[1]shot analysis'!AC30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30" t="e">
+        <f>'[1]shot analysis'!AD30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L30" t="e">
+        <f>[1]portcullis!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M30" t="e">
+        <f>'[1]cheval de frise'!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N30" t="e">
+        <f>[1]moat!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O30" t="e">
+        <f>[1]ramparts!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P30" t="e">
+        <f>[1]drawbridge!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q30" t="e">
+        <f>'[1]sally port'!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R30" t="e">
+        <f>'[1]rock wall'!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S30" t="e">
+        <f>'[1]rough terrain'!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T30" t="e">
+        <f>[1]lowbar!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V30" t="e">
+        <f>[1]climb!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W30" t="e">
+        <f>[1]rip!L29</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="e">
+        <f>'[1]shot analysis'!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C31" t="e">
+        <f>'[1]shot analysis'!M31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D31" t="e">
+        <f>'[1]shot analysis'!N31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E31" t="e">
+        <f>'[1]shot analysis'!O31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G31" t="e">
+        <f>'[1]shot analysis'!AA31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" t="e">
+        <f>'[1]shot analysis'!AB31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" t="e">
+        <f>'[1]shot analysis'!AC31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J31" t="e">
+        <f>'[1]shot analysis'!AD31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L31" t="e">
+        <f>[1]portcullis!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M31" t="e">
+        <f>'[1]cheval de frise'!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N31" t="e">
+        <f>[1]moat!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O31" t="e">
+        <f>[1]ramparts!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P31" t="e">
+        <f>[1]drawbridge!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q31" t="e">
+        <f>'[1]sally port'!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R31" t="e">
+        <f>'[1]rock wall'!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S31" t="e">
+        <f>'[1]rough terrain'!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T31" t="e">
+        <f>[1]lowbar!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V31" t="e">
+        <f>[1]climb!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W31" t="e">
+        <f>[1]rip!L30</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="e">
+        <f>'[1]shot analysis'!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C32" t="e">
+        <f>'[1]shot analysis'!M32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D32" t="e">
+        <f>'[1]shot analysis'!N32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E32" t="e">
+        <f>'[1]shot analysis'!O32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G32" t="e">
+        <f>'[1]shot analysis'!AA32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" t="e">
+        <f>'[1]shot analysis'!AB32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" t="e">
+        <f>'[1]shot analysis'!AC32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J32" t="e">
+        <f>'[1]shot analysis'!AD32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L32" t="e">
+        <f>[1]portcullis!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M32" t="e">
+        <f>'[1]cheval de frise'!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N32" t="e">
+        <f>[1]moat!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O32" t="e">
+        <f>[1]ramparts!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P32" t="e">
+        <f>[1]drawbridge!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q32" t="e">
+        <f>'[1]sally port'!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R32" t="e">
+        <f>'[1]rock wall'!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S32" t="e">
+        <f>'[1]rough terrain'!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T32" t="e">
+        <f>[1]lowbar!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V32" t="e">
+        <f>[1]climb!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W32" t="e">
+        <f>[1]rip!L31</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="e">
+        <f>'[1]shot analysis'!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C33" t="e">
+        <f>'[1]shot analysis'!M33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D33" t="e">
+        <f>'[1]shot analysis'!N33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E33" t="e">
+        <f>'[1]shot analysis'!O33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G33" t="e">
+        <f>'[1]shot analysis'!AA33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" t="e">
+        <f>'[1]shot analysis'!AB33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" t="e">
+        <f>'[1]shot analysis'!AC33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J33" t="e">
+        <f>'[1]shot analysis'!AD33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L33" t="e">
+        <f>[1]portcullis!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33" t="e">
+        <f>'[1]cheval de frise'!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N33" t="e">
+        <f>[1]moat!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O33" t="e">
+        <f>[1]ramparts!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P33" t="e">
+        <f>[1]drawbridge!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q33" t="e">
+        <f>'[1]sally port'!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R33" t="e">
+        <f>'[1]rock wall'!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S33" t="e">
+        <f>'[1]rough terrain'!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T33" t="e">
+        <f>[1]lowbar!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V33" t="e">
+        <f>[1]climb!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W33" t="e">
+        <f>[1]rip!L32</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="e">
+        <f>'[1]shot analysis'!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C34" t="e">
+        <f>'[1]shot analysis'!M34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D34" t="e">
+        <f>'[1]shot analysis'!N34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E34" t="e">
+        <f>'[1]shot analysis'!O34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G34" t="e">
+        <f>'[1]shot analysis'!AA34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" t="e">
+        <f>'[1]shot analysis'!AB34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" t="e">
+        <f>'[1]shot analysis'!AC34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J34" t="e">
+        <f>'[1]shot analysis'!AD34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L34" t="e">
+        <f>[1]portcullis!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M34" t="e">
+        <f>'[1]cheval de frise'!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N34" t="e">
+        <f>[1]moat!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O34" t="e">
+        <f>[1]ramparts!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P34" t="e">
+        <f>[1]drawbridge!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q34" t="e">
+        <f>'[1]sally port'!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R34" t="e">
+        <f>'[1]rock wall'!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S34" t="e">
+        <f>'[1]rough terrain'!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T34" t="e">
+        <f>[1]lowbar!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V34" t="e">
+        <f>[1]climb!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W34" t="e">
+        <f>[1]rip!L33</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="e">
+        <f>'[1]shot analysis'!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C35" t="e">
+        <f>'[1]shot analysis'!M35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D35" t="e">
+        <f>'[1]shot analysis'!N35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E35" t="e">
+        <f>'[1]shot analysis'!O35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G35" t="e">
+        <f>'[1]shot analysis'!AA35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" t="e">
+        <f>'[1]shot analysis'!AB35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" t="e">
+        <f>'[1]shot analysis'!AC35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J35" t="e">
+        <f>'[1]shot analysis'!AD35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L35" t="e">
+        <f>[1]portcullis!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" t="e">
+        <f>'[1]cheval de frise'!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N35" t="e">
+        <f>[1]moat!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O35" t="e">
+        <f>[1]ramparts!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P35" t="e">
+        <f>[1]drawbridge!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q35" t="e">
+        <f>'[1]sally port'!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R35" t="e">
+        <f>'[1]rock wall'!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S35" t="e">
+        <f>'[1]rough terrain'!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T35" t="e">
+        <f>[1]lowbar!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V35" t="e">
+        <f>[1]climb!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W35" t="e">
+        <f>[1]rip!L34</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="e">
+        <f>'[1]shot analysis'!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C36" t="e">
+        <f>'[1]shot analysis'!M36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D36" t="e">
+        <f>'[1]shot analysis'!N36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E36" t="e">
+        <f>'[1]shot analysis'!O36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G36" t="e">
+        <f>'[1]shot analysis'!AA36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H36" t="e">
+        <f>'[1]shot analysis'!AB36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" t="e">
+        <f>'[1]shot analysis'!AC36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J36" t="e">
+        <f>'[1]shot analysis'!AD36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L36" t="e">
+        <f>[1]portcullis!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M36" t="e">
+        <f>'[1]cheval de frise'!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N36" t="e">
+        <f>[1]moat!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O36" t="e">
+        <f>[1]ramparts!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P36" t="e">
+        <f>[1]drawbridge!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q36" t="e">
+        <f>'[1]sally port'!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R36" t="e">
+        <f>'[1]rock wall'!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S36" t="e">
+        <f>'[1]rough terrain'!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T36" t="e">
+        <f>[1]lowbar!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V36" t="e">
+        <f>[1]climb!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W36" t="e">
+        <f>[1]rip!L35</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="e">
+        <f>'[1]shot analysis'!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C37" t="e">
+        <f>'[1]shot analysis'!M37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D37" t="e">
+        <f>'[1]shot analysis'!N37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E37" t="e">
+        <f>'[1]shot analysis'!O37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G37" t="e">
+        <f>'[1]shot analysis'!AA37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H37" t="e">
+        <f>'[1]shot analysis'!AB37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" t="e">
+        <f>'[1]shot analysis'!AC37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J37" t="e">
+        <f>'[1]shot analysis'!AD37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L37" t="e">
+        <f>[1]portcullis!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M37" t="e">
+        <f>'[1]cheval de frise'!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N37" t="e">
+        <f>[1]moat!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O37" t="e">
+        <f>[1]ramparts!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P37" t="e">
+        <f>[1]drawbridge!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q37" t="e">
+        <f>'[1]sally port'!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R37" t="e">
+        <f>'[1]rock wall'!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S37" t="e">
+        <f>'[1]rough terrain'!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T37" t="e">
+        <f>[1]lowbar!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V37" t="e">
+        <f>[1]climb!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W37" t="e">
+        <f>[1]rip!L36</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="e">
+        <f>'[1]shot analysis'!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C38" t="e">
+        <f>'[1]shot analysis'!M38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D38" t="e">
+        <f>'[1]shot analysis'!N38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E38" t="e">
+        <f>'[1]shot analysis'!O38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G38" t="e">
+        <f>'[1]shot analysis'!AA38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" t="e">
+        <f>'[1]shot analysis'!AB38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" t="e">
+        <f>'[1]shot analysis'!AC38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J38" t="e">
+        <f>'[1]shot analysis'!AD38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L38" t="e">
+        <f>[1]portcullis!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M38" t="e">
+        <f>'[1]cheval de frise'!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N38" t="e">
+        <f>[1]moat!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O38" t="e">
+        <f>[1]ramparts!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P38" t="e">
+        <f>[1]drawbridge!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q38" t="e">
+        <f>'[1]sally port'!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R38" t="e">
+        <f>'[1]rock wall'!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S38" t="e">
+        <f>'[1]rough terrain'!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T38" t="e">
+        <f>[1]lowbar!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V38" t="e">
+        <f>[1]climb!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W38" t="e">
+        <f>[1]rip!L37</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="e">
+        <f>'[1]shot analysis'!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C39" t="e">
+        <f>'[1]shot analysis'!M39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D39" t="e">
+        <f>'[1]shot analysis'!N39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E39" t="e">
+        <f>'[1]shot analysis'!O39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G39" t="e">
+        <f>'[1]shot analysis'!AA39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H39" t="e">
+        <f>'[1]shot analysis'!AB39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" t="e">
+        <f>'[1]shot analysis'!AC39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J39" t="e">
+        <f>'[1]shot analysis'!AD39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L39" t="e">
+        <f>[1]portcullis!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M39" t="e">
+        <f>'[1]cheval de frise'!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N39" t="e">
+        <f>[1]moat!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O39" t="e">
+        <f>[1]ramparts!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P39" t="e">
+        <f>[1]drawbridge!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q39" t="e">
+        <f>'[1]sally port'!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R39" t="e">
+        <f>'[1]rock wall'!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S39" t="e">
+        <f>'[1]rough terrain'!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T39" t="e">
+        <f>[1]lowbar!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V39" t="e">
+        <f>[1]climb!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W39" t="e">
+        <f>[1]rip!L38</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="e">
+        <f>'[1]shot analysis'!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C40" t="e">
+        <f>'[1]shot analysis'!M40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D40" t="e">
+        <f>'[1]shot analysis'!N40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E40" t="e">
+        <f>'[1]shot analysis'!O40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G40" t="e">
+        <f>'[1]shot analysis'!AA40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" t="e">
+        <f>'[1]shot analysis'!AB40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" t="e">
+        <f>'[1]shot analysis'!AC40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J40" t="e">
+        <f>'[1]shot analysis'!AD40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L40" t="e">
+        <f>[1]portcullis!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M40" t="e">
+        <f>'[1]cheval de frise'!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N40" t="e">
+        <f>[1]moat!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O40" t="e">
+        <f>[1]ramparts!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P40" t="e">
+        <f>[1]drawbridge!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q40" t="e">
+        <f>'[1]sally port'!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R40" t="e">
+        <f>'[1]rock wall'!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S40" t="e">
+        <f>'[1]rough terrain'!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T40" t="e">
+        <f>[1]lowbar!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V40" t="e">
+        <f>[1]climb!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W40" t="e">
+        <f>[1]rip!L39</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="e">
+        <f>'[1]shot analysis'!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C41" t="e">
+        <f>'[1]shot analysis'!M41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D41" t="e">
+        <f>'[1]shot analysis'!N41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E41" t="e">
+        <f>'[1]shot analysis'!O41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G41" t="e">
+        <f>'[1]shot analysis'!AA41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" t="e">
+        <f>'[1]shot analysis'!AB41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" t="e">
+        <f>'[1]shot analysis'!AC41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J41" t="e">
+        <f>'[1]shot analysis'!AD41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L41" t="e">
+        <f>[1]portcullis!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M41" t="e">
+        <f>'[1]cheval de frise'!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N41" t="e">
+        <f>[1]moat!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O41" t="e">
+        <f>[1]ramparts!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P41" t="e">
+        <f>[1]drawbridge!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q41" t="e">
+        <f>'[1]sally port'!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R41" t="e">
+        <f>'[1]rock wall'!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S41" t="e">
+        <f>'[1]rough terrain'!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T41" t="e">
+        <f>[1]lowbar!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V41" t="e">
+        <f>[1]climb!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W41" t="e">
+        <f>[1]rip!L40</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="e">
+        <f>'[1]shot analysis'!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C42" t="e">
+        <f>'[1]shot analysis'!M42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D42" t="e">
+        <f>'[1]shot analysis'!N42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E42" t="e">
+        <f>'[1]shot analysis'!O42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G42" t="e">
+        <f>'[1]shot analysis'!AA42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H42" t="e">
+        <f>'[1]shot analysis'!AB42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" t="e">
+        <f>'[1]shot analysis'!AC42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J42" t="e">
+        <f>'[1]shot analysis'!AD42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L42" t="e">
+        <f>[1]portcullis!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M42" t="e">
+        <f>'[1]cheval de frise'!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N42" t="e">
+        <f>[1]moat!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O42" t="e">
+        <f>[1]ramparts!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P42" t="e">
+        <f>[1]drawbridge!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q42" t="e">
+        <f>'[1]sally port'!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R42" t="e">
+        <f>'[1]rock wall'!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S42" t="e">
+        <f>'[1]rough terrain'!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T42" t="e">
+        <f>[1]lowbar!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V42" t="e">
+        <f>[1]climb!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W42" t="e">
+        <f>[1]rip!L41</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="e">
+        <f>'[1]shot analysis'!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C43" t="e">
+        <f>'[1]shot analysis'!M43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D43" t="e">
+        <f>'[1]shot analysis'!N43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E43" t="e">
+        <f>'[1]shot analysis'!O43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G43" t="e">
+        <f>'[1]shot analysis'!AA43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H43" t="e">
+        <f>'[1]shot analysis'!AB43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" t="e">
+        <f>'[1]shot analysis'!AC43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J43" t="e">
+        <f>'[1]shot analysis'!AD43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L43" t="e">
+        <f>[1]portcullis!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M43" t="e">
+        <f>'[1]cheval de frise'!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N43" t="e">
+        <f>[1]moat!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O43" t="e">
+        <f>[1]ramparts!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P43" t="e">
+        <f>[1]drawbridge!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q43" t="e">
+        <f>'[1]sally port'!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R43" t="e">
+        <f>'[1]rock wall'!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S43" t="e">
+        <f>'[1]rough terrain'!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T43" t="e">
+        <f>[1]lowbar!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V43" t="e">
+        <f>[1]climb!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W43" t="e">
+        <f>[1]rip!L42</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="e">
+        <f>'[1]shot analysis'!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C44" t="e">
+        <f>'[1]shot analysis'!M44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D44" t="e">
+        <f>'[1]shot analysis'!N44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E44" t="e">
+        <f>'[1]shot analysis'!O44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G44" t="e">
+        <f>'[1]shot analysis'!AA44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H44" t="e">
+        <f>'[1]shot analysis'!AB44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I44" t="e">
+        <f>'[1]shot analysis'!AC44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J44" t="e">
+        <f>'[1]shot analysis'!AD44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L44" t="e">
+        <f>[1]portcullis!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M44" t="e">
+        <f>'[1]cheval de frise'!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N44" t="e">
+        <f>[1]moat!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O44" t="e">
+        <f>[1]ramparts!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P44" t="e">
+        <f>[1]drawbridge!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q44" t="e">
+        <f>'[1]sally port'!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R44" t="e">
+        <f>'[1]rock wall'!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S44" t="e">
+        <f>'[1]rough terrain'!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T44" t="e">
+        <f>[1]lowbar!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V44" t="e">
+        <f>[1]climb!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W44" t="e">
+        <f>[1]rip!L43</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="e">
+        <f>'[1]shot analysis'!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C45" t="e">
+        <f>'[1]shot analysis'!M45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D45" t="e">
+        <f>'[1]shot analysis'!N45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E45" t="e">
+        <f>'[1]shot analysis'!O45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G45" t="e">
+        <f>'[1]shot analysis'!AA45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H45" t="e">
+        <f>'[1]shot analysis'!AB45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I45" t="e">
+        <f>'[1]shot analysis'!AC45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J45" t="e">
+        <f>'[1]shot analysis'!AD45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L45" t="e">
+        <f>[1]portcullis!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M45" t="e">
+        <f>'[1]cheval de frise'!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N45" t="e">
+        <f>[1]moat!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O45" t="e">
+        <f>[1]ramparts!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P45" t="e">
+        <f>[1]drawbridge!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q45" t="e">
+        <f>'[1]sally port'!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R45" t="e">
+        <f>'[1]rock wall'!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S45" t="e">
+        <f>'[1]rough terrain'!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T45" t="e">
+        <f>[1]lowbar!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V45" t="e">
+        <f>[1]climb!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W45" t="e">
+        <f>[1]rip!L44</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="e">
+        <f>'[1]shot analysis'!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C46" t="e">
+        <f>'[1]shot analysis'!M46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D46" t="e">
+        <f>'[1]shot analysis'!N46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E46" t="e">
+        <f>'[1]shot analysis'!O46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46" t="e">
+        <f>'[1]shot analysis'!AA46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H46" t="e">
+        <f>'[1]shot analysis'!AB46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I46" t="e">
+        <f>'[1]shot analysis'!AC46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J46" t="e">
+        <f>'[1]shot analysis'!AD46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L46" t="e">
+        <f>[1]portcullis!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M46" t="e">
+        <f>'[1]cheval de frise'!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N46" t="e">
+        <f>[1]moat!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O46" t="e">
+        <f>[1]ramparts!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P46" t="e">
+        <f>[1]drawbridge!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q46" t="e">
+        <f>'[1]sally port'!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R46" t="e">
+        <f>'[1]rock wall'!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S46" t="e">
+        <f>'[1]rough terrain'!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T46" t="e">
+        <f>[1]lowbar!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V46" t="e">
+        <f>[1]climb!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W46" t="e">
+        <f>[1]rip!L45</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="e">
+        <f>'[1]shot analysis'!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C47" t="e">
+        <f>'[1]shot analysis'!M47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D47" t="e">
+        <f>'[1]shot analysis'!N47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E47" t="e">
+        <f>'[1]shot analysis'!O47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47" t="e">
+        <f>'[1]shot analysis'!AA47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H47" t="e">
+        <f>'[1]shot analysis'!AB47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I47" t="e">
+        <f>'[1]shot analysis'!AC47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J47" t="e">
+        <f>'[1]shot analysis'!AD47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" t="e">
+        <f>[1]portcullis!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M47" t="e">
+        <f>'[1]cheval de frise'!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N47" t="e">
+        <f>[1]moat!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O47" t="e">
+        <f>[1]ramparts!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P47" t="e">
+        <f>[1]drawbridge!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q47" t="e">
+        <f>'[1]sally port'!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R47" t="e">
+        <f>'[1]rock wall'!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S47" t="e">
+        <f>'[1]rough terrain'!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T47" t="e">
+        <f>[1]lowbar!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V47" t="e">
+        <f>[1]climb!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W47" t="e">
+        <f>[1]rip!L46</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="e">
+        <f>'[1]shot analysis'!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C48" t="e">
+        <f>'[1]shot analysis'!M48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D48" t="e">
+        <f>'[1]shot analysis'!N48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E48" t="e">
+        <f>'[1]shot analysis'!O48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G48" t="e">
+        <f>'[1]shot analysis'!AA48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H48" t="e">
+        <f>'[1]shot analysis'!AB48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I48" t="e">
+        <f>'[1]shot analysis'!AC48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J48" t="e">
+        <f>'[1]shot analysis'!AD48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L48" t="e">
+        <f>[1]portcullis!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M48" t="e">
+        <f>'[1]cheval de frise'!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N48" t="e">
+        <f>[1]moat!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O48" t="e">
+        <f>[1]ramparts!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P48" t="e">
+        <f>[1]drawbridge!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q48" t="e">
+        <f>'[1]sally port'!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R48" t="e">
+        <f>'[1]rock wall'!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S48" t="e">
+        <f>'[1]rough terrain'!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T48" t="e">
+        <f>[1]lowbar!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V48" t="e">
+        <f>[1]climb!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W48" t="e">
+        <f>[1]rip!L47</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="e">
+        <f>'[1]shot analysis'!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C49" t="e">
+        <f>'[1]shot analysis'!M49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D49" t="e">
+        <f>'[1]shot analysis'!N49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E49" t="e">
+        <f>'[1]shot analysis'!O49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G49" t="e">
+        <f>'[1]shot analysis'!AA49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H49" t="e">
+        <f>'[1]shot analysis'!AB49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I49" t="e">
+        <f>'[1]shot analysis'!AC49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J49" t="e">
+        <f>'[1]shot analysis'!AD49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L49" t="e">
+        <f>[1]portcullis!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M49" t="e">
+        <f>'[1]cheval de frise'!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N49" t="e">
+        <f>[1]moat!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O49" t="e">
+        <f>[1]ramparts!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P49" t="e">
+        <f>[1]drawbridge!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q49" t="e">
+        <f>'[1]sally port'!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R49" t="e">
+        <f>'[1]rock wall'!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S49" t="e">
+        <f>'[1]rough terrain'!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T49" t="e">
+        <f>[1]lowbar!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V49" t="e">
+        <f>[1]climb!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W49" t="e">
+        <f>[1]rip!L48</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="e">
+        <f>'[1]shot analysis'!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C50" t="e">
+        <f>'[1]shot analysis'!M50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D50" t="e">
+        <f>'[1]shot analysis'!N50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E50" t="e">
+        <f>'[1]shot analysis'!O50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G50" t="e">
+        <f>'[1]shot analysis'!AA50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H50" t="e">
+        <f>'[1]shot analysis'!AB50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I50" t="e">
+        <f>'[1]shot analysis'!AC50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J50" t="e">
+        <f>'[1]shot analysis'!AD50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L50" t="e">
+        <f>[1]portcullis!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M50" t="e">
+        <f>'[1]cheval de frise'!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N50" t="e">
+        <f>[1]moat!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O50" t="e">
+        <f>[1]ramparts!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P50" t="e">
+        <f>[1]drawbridge!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q50" t="e">
+        <f>'[1]sally port'!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R50" t="e">
+        <f>'[1]rock wall'!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S50" t="e">
+        <f>'[1]rough terrain'!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T50" t="e">
+        <f>[1]lowbar!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V50" t="e">
+        <f>[1]climb!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W50" t="e">
+        <f>[1]rip!L49</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="e">
+        <f>'[1]shot analysis'!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C51" t="e">
+        <f>'[1]shot analysis'!M51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D51" t="e">
+        <f>'[1]shot analysis'!N51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E51" t="e">
+        <f>'[1]shot analysis'!O51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G51" t="e">
+        <f>'[1]shot analysis'!AA51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H51" t="e">
+        <f>'[1]shot analysis'!AB51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I51" t="e">
+        <f>'[1]shot analysis'!AC51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J51" t="e">
+        <f>'[1]shot analysis'!AD51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L51" t="e">
+        <f>[1]portcullis!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M51" t="e">
+        <f>'[1]cheval de frise'!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N51" t="e">
+        <f>[1]moat!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O51" t="e">
+        <f>[1]ramparts!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P51" t="e">
+        <f>[1]drawbridge!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q51" t="e">
+        <f>'[1]sally port'!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R51" t="e">
+        <f>'[1]rock wall'!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S51" t="e">
+        <f>'[1]rough terrain'!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T51" t="e">
+        <f>[1]lowbar!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V51" t="e">
+        <f>[1]climb!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W51" t="e">
+        <f>[1]rip!L50</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="e">
+        <f>'[1]shot analysis'!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C52" t="e">
+        <f>'[1]shot analysis'!M52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D52" t="e">
+        <f>'[1]shot analysis'!N52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E52" t="e">
+        <f>'[1]shot analysis'!O52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G52" t="e">
+        <f>'[1]shot analysis'!AA52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H52" t="e">
+        <f>'[1]shot analysis'!AB52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I52" t="e">
+        <f>'[1]shot analysis'!AC52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J52" t="e">
+        <f>'[1]shot analysis'!AD52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L52" t="e">
+        <f>[1]portcullis!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M52" t="e">
+        <f>'[1]cheval de frise'!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N52" t="e">
+        <f>[1]moat!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O52" t="e">
+        <f>[1]ramparts!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P52" t="e">
+        <f>[1]drawbridge!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q52" t="e">
+        <f>'[1]sally port'!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R52" t="e">
+        <f>'[1]rock wall'!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S52" t="e">
+        <f>'[1]rough terrain'!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T52" t="e">
+        <f>[1]lowbar!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V52" t="e">
+        <f>[1]climb!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W52" t="e">
+        <f>[1]rip!L51</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="e">
+        <f>'[1]shot analysis'!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C53" t="e">
+        <f>'[1]shot analysis'!M53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D53" t="e">
+        <f>'[1]shot analysis'!N53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E53" t="e">
+        <f>'[1]shot analysis'!O53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G53" t="e">
+        <f>'[1]shot analysis'!AA53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H53" t="e">
+        <f>'[1]shot analysis'!AB53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I53" t="e">
+        <f>'[1]shot analysis'!AC53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J53" t="e">
+        <f>'[1]shot analysis'!AD53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L53" t="e">
+        <f>[1]portcullis!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M53" t="e">
+        <f>'[1]cheval de frise'!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N53" t="e">
+        <f>[1]moat!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O53" t="e">
+        <f>[1]ramparts!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P53" t="e">
+        <f>[1]drawbridge!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q53" t="e">
+        <f>'[1]sally port'!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R53" t="e">
+        <f>'[1]rock wall'!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S53" t="e">
+        <f>'[1]rough terrain'!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T53" t="e">
+        <f>[1]lowbar!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V53" t="e">
+        <f>[1]climb!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W53" t="e">
+        <f>[1]rip!L52</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="e">
+        <f>'[1]shot analysis'!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C54" t="e">
+        <f>'[1]shot analysis'!M54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D54" t="e">
+        <f>'[1]shot analysis'!N54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E54" t="e">
+        <f>'[1]shot analysis'!O54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G54" t="e">
+        <f>'[1]shot analysis'!AA54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H54" t="e">
+        <f>'[1]shot analysis'!AB54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I54" t="e">
+        <f>'[1]shot analysis'!AC54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J54" t="e">
+        <f>'[1]shot analysis'!AD54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L54" t="e">
+        <f>[1]portcullis!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M54" t="e">
+        <f>'[1]cheval de frise'!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N54" t="e">
+        <f>[1]moat!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O54" t="e">
+        <f>[1]ramparts!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P54" t="e">
+        <f>[1]drawbridge!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q54" t="e">
+        <f>'[1]sally port'!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R54" t="e">
+        <f>'[1]rock wall'!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S54" t="e">
+        <f>'[1]rough terrain'!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T54" t="e">
+        <f>[1]lowbar!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V54" t="e">
+        <f>[1]climb!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W54" t="e">
+        <f>[1]rip!L53</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="e">
+        <f>'[1]shot analysis'!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C55" t="e">
+        <f>'[1]shot analysis'!M55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D55" t="e">
+        <f>'[1]shot analysis'!N55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E55" t="e">
+        <f>'[1]shot analysis'!O55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G55" t="e">
+        <f>'[1]shot analysis'!AA55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H55" t="e">
+        <f>'[1]shot analysis'!AB55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I55" t="e">
+        <f>'[1]shot analysis'!AC55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J55" t="e">
+        <f>'[1]shot analysis'!AD55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L55" t="e">
+        <f>[1]portcullis!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M55" t="e">
+        <f>'[1]cheval de frise'!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N55" t="e">
+        <f>[1]moat!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O55" t="e">
+        <f>[1]ramparts!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P55" t="e">
+        <f>[1]drawbridge!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q55" t="e">
+        <f>'[1]sally port'!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R55" t="e">
+        <f>'[1]rock wall'!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S55" t="e">
+        <f>'[1]rough terrain'!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T55" t="e">
+        <f>[1]lowbar!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V55" t="e">
+        <f>[1]climb!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W55" t="e">
+        <f>[1]rip!L54</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="e">
+        <f>'[1]shot analysis'!L56</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C56" t="e">
+        <f>'[1]shot analysis'!M56</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D56" t="e">
+        <f>'[1]shot analysis'!N56</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E56" t="e">
+        <f>'[1]shot analysis'!O56</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G56" t="e">
+        <f>'[1]shot analysis'!AA56</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H56" t="e">
+        <f>'[1]shot analysis'!AB56</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I56" t="e">
+        <f>'[1]shot analysis'!AC56</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J56" t="e">
+        <f>'[1]shot analysis'!AD56</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L56" t="e">
+        <f>[1]portcullis!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M56" t="e">
+        <f>'[1]cheval de frise'!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N56" t="e">
+        <f>[1]moat!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O56" t="e">
+        <f>[1]ramparts!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P56" t="e">
+        <f>[1]drawbridge!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q56" t="e">
+        <f>'[1]sally port'!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R56" t="e">
+        <f>'[1]rock wall'!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S56" t="e">
+        <f>'[1]rough terrain'!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T56" t="e">
+        <f>[1]lowbar!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V56" t="e">
+        <f>[1]climb!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W56" t="e">
+        <f>[1]rip!L55</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>